<commit_message>
DDL e DML Finalizadas
</commit_message>
<xml_diff>
--- a/Modelagens/Modelagens_SpMedGroup-Físico.xlsx
+++ b/Modelagens/Modelagens_SpMedGroup-Físico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livia\OneDrive\Documents\Lívia\Lívia Escola\SENAI\sprint-1-bd\exercicios\SpMedGroup\Modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB4BE0F1-FF15-4CC8-B127-EBD15BFEF2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FBE86CE-77B1-4AB3-B4B0-21511F2093D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{03839324-049D-4BCD-8CB4-4926F755280E}"/>
+    <workbookView xWindow="14250" yWindow="3810" windowWidth="15375" windowHeight="6090" xr2:uid="{03839324-049D-4BCD-8CB4-4926F755280E}"/>
   </bookViews>
   <sheets>
     <sheet name="Físico" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="135">
   <si>
     <t>TipoUsuario</t>
   </si>
@@ -427,6 +427,18 @@
   </si>
   <si>
     <t>SP Medical Group</t>
+  </si>
+  <si>
+    <t>Vila Mariana</t>
+  </si>
+  <si>
+    <t>01202-001</t>
+  </si>
+  <si>
+    <t>8:00 -19:00</t>
+  </si>
+  <si>
+    <t>Campos Elíseos</t>
   </si>
 </sst>
 </file>
@@ -458,7 +470,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,6 +609,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -663,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -671,168 +689,180 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1160,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CE33BF-5118-4F54-98F8-364B9B925BD9}">
   <dimension ref="B2:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="H31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K48" sqref="K48:L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,584 +1211,602 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="F2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="M2" s="19" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="M2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="21"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="54"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="F3" s="11" t="s">
+      <c r="D3" s="58"/>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
+      <c r="H3" s="24"/>
+      <c r="I3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="11" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="22" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="29"/>
-      <c r="S3" s="28" t="s">
+      <c r="R3" s="51"/>
+      <c r="S3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="29"/>
-      <c r="U3" s="28" t="s">
+      <c r="T3" s="51"/>
+      <c r="U3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="29"/>
-      <c r="W3" s="28" t="s">
+      <c r="V3" s="51"/>
+      <c r="W3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="29"/>
+      <c r="X3" s="51"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="F4" s="13">
+      <c r="D4" s="56"/>
+      <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="33">
         <v>1</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="16" t="s">
+      <c r="H4" s="33"/>
+      <c r="I4" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="14"/>
-      <c r="K4" s="13">
+      <c r="J4" s="33"/>
+      <c r="K4" s="5">
         <v>123</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="9">
         <v>1</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="9">
         <v>6</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="9">
         <v>2</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="P4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="43">
         <v>30602</v>
       </c>
-      <c r="R4" s="27"/>
-      <c r="S4" s="24" t="s">
+      <c r="R4" s="44"/>
+      <c r="S4" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="25"/>
-      <c r="U4" s="24">
+      <c r="T4" s="47"/>
+      <c r="U4" s="46">
         <v>432124576</v>
       </c>
-      <c r="V4" s="25"/>
-      <c r="W4" s="24">
+      <c r="V4" s="47"/>
+      <c r="W4" s="46">
         <v>94839859000</v>
       </c>
-      <c r="X4" s="25"/>
+      <c r="X4" s="47"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="F5" s="13">
+      <c r="D5" s="56"/>
+      <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="33">
         <v>1</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="16" t="s">
+      <c r="H5" s="33"/>
+      <c r="I5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="13">
-        <v>132</v>
-      </c>
-      <c r="M5" s="23">
+      <c r="J5" s="33"/>
+      <c r="K5" s="5">
+        <v>345</v>
+      </c>
+      <c r="M5" s="9">
         <v>2</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="9">
         <v>7</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="9">
         <v>3</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="43">
         <v>37095</v>
       </c>
-      <c r="R5" s="27"/>
-      <c r="S5" s="24" t="s">
+      <c r="R5" s="44"/>
+      <c r="S5" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="25"/>
-      <c r="U5" s="24" t="s">
+      <c r="T5" s="47"/>
+      <c r="U5" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="25"/>
-      <c r="W5" s="24">
+      <c r="V5" s="47"/>
+      <c r="W5" s="46">
         <v>73556944057</v>
       </c>
-      <c r="X5" s="25"/>
+      <c r="X5" s="47"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="F6" s="13">
+      <c r="D6" s="56"/>
+      <c r="F6" s="5">
         <v>3</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="33">
         <v>2</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="16" t="s">
+      <c r="H6" s="33"/>
+      <c r="I6" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="14"/>
-      <c r="K6" s="13">
-        <v>167</v>
-      </c>
-      <c r="M6" s="23">
+      <c r="J6" s="33"/>
+      <c r="K6" s="5">
+        <v>567</v>
+      </c>
+      <c r="M6" s="9">
         <v>3</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="9">
         <v>8</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="9">
         <v>4</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="43">
         <v>28773</v>
       </c>
-      <c r="R6" s="27"/>
-      <c r="S6" s="24" t="s">
+      <c r="R6" s="44"/>
+      <c r="S6" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="T6" s="25"/>
-      <c r="U6" s="24" t="s">
+      <c r="T6" s="47"/>
+      <c r="U6" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="V6" s="25"/>
-      <c r="W6" s="24">
+      <c r="V6" s="47"/>
+      <c r="W6" s="46">
         <v>16839338002</v>
       </c>
-      <c r="X6" s="25"/>
+      <c r="X6" s="47"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F7" s="13">
+      <c r="F7" s="5">
         <v>4</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="33">
         <v>2</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="16" t="s">
+      <c r="H7" s="33"/>
+      <c r="I7" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="14"/>
-      <c r="K7" s="13"/>
-      <c r="M7" s="23">
+      <c r="J7" s="33"/>
+      <c r="K7" s="5">
+        <v>789</v>
+      </c>
+      <c r="M7" s="9">
         <v>4</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="9">
         <v>9</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="9">
         <v>5</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="43">
         <v>31333</v>
       </c>
-      <c r="R7" s="27"/>
-      <c r="S7" s="24" t="s">
+      <c r="R7" s="44"/>
+      <c r="S7" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="25"/>
-      <c r="U7" s="24" t="s">
+      <c r="T7" s="47"/>
+      <c r="U7" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="V7" s="25"/>
-      <c r="W7" s="24">
+      <c r="V7" s="47"/>
+      <c r="W7" s="46">
         <v>14332654765</v>
       </c>
-      <c r="X7" s="25"/>
+      <c r="X7" s="47"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F8" s="13">
+      <c r="F8" s="5">
         <v>5</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="33">
         <v>2</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="16" t="s">
+      <c r="H8" s="33"/>
+      <c r="I8" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="13"/>
-      <c r="M8" s="23">
+      <c r="J8" s="33"/>
+      <c r="K8" s="5">
+        <v>910</v>
+      </c>
+      <c r="M8" s="9">
         <v>5</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="9">
         <v>10</v>
       </c>
-      <c r="O8" s="23">
+      <c r="O8" s="9">
         <v>6</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="43">
         <v>27633</v>
       </c>
-      <c r="R8" s="27"/>
-      <c r="S8" s="24" t="s">
+      <c r="R8" s="44"/>
+      <c r="S8" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="T8" s="25"/>
-      <c r="U8" s="24" t="s">
+      <c r="T8" s="47"/>
+      <c r="U8" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="V8" s="25"/>
-      <c r="W8" s="24">
+      <c r="V8" s="47"/>
+      <c r="W8" s="46">
         <v>91305348010</v>
       </c>
-      <c r="X8" s="25"/>
+      <c r="X8" s="47"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F9" s="13">
+      <c r="F9" s="5">
         <v>6</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="33">
         <v>3</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="16" t="s">
+      <c r="H9" s="33"/>
+      <c r="I9" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="13"/>
-      <c r="M9" s="23">
+      <c r="J9" s="33"/>
+      <c r="K9" s="5">
+        <v>101</v>
+      </c>
+      <c r="M9" s="9">
         <v>6</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="9">
         <v>11</v>
       </c>
-      <c r="O9" s="23">
+      <c r="O9" s="9">
         <v>7</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="P9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="26">
+      <c r="Q9" s="43">
         <v>26379</v>
       </c>
-      <c r="R9" s="27"/>
-      <c r="S9" s="24" t="s">
+      <c r="R9" s="44"/>
+      <c r="S9" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="T9" s="25"/>
-      <c r="U9" s="24" t="s">
+      <c r="T9" s="47"/>
+      <c r="U9" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="V9" s="25"/>
-      <c r="W9" s="24">
+      <c r="V9" s="47"/>
+      <c r="W9" s="46">
         <v>79799299004</v>
       </c>
-      <c r="X9" s="25"/>
+      <c r="X9" s="47"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F10" s="13">
+      <c r="F10" s="5">
         <v>7</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="33">
         <v>3</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="16" t="s">
+      <c r="H10" s="33"/>
+      <c r="I10" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="13"/>
-      <c r="M10" s="23">
+      <c r="J10" s="33"/>
+      <c r="K10" s="5">
+        <v>102</v>
+      </c>
+      <c r="M10" s="9">
         <v>7</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="9">
         <v>12</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="9">
         <v>8</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="26">
+      <c r="Q10" s="43">
         <v>43164</v>
       </c>
-      <c r="R10" s="27"/>
-      <c r="S10" s="24"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="24" t="s">
+      <c r="R10" s="44"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="V10" s="25"/>
-      <c r="W10" s="24">
+      <c r="V10" s="47"/>
+      <c r="W10" s="46">
         <v>13771913039</v>
       </c>
-      <c r="X10" s="25"/>
+      <c r="X10" s="47"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="13">
+      <c r="F11" s="5">
         <v>8</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="33">
         <v>3</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="16" t="s">
+      <c r="H11" s="33"/>
+      <c r="I11" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="14"/>
-      <c r="K11" s="13"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="5">
+        <v>103</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F12" s="13">
+      <c r="F12" s="5">
         <v>9</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="33">
         <v>3</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="16" t="s">
+      <c r="H12" s="33"/>
+      <c r="I12" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="14"/>
-      <c r="K12" s="13"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="5">
+        <v>104</v>
+      </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="13">
+      <c r="F13" s="5">
         <v>10</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="33">
         <v>3</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="16" t="s">
+      <c r="H13" s="33"/>
+      <c r="I13" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="14"/>
-      <c r="K13" s="13"/>
-      <c r="M13" s="31" t="s">
+      <c r="J13" s="33"/>
+      <c r="K13" s="5">
+        <v>105</v>
+      </c>
+      <c r="M13" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="31"/>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
+      <c r="N13" s="45"/>
+      <c r="O13" s="45"/>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F14" s="13">
+      <c r="F14" s="5">
         <v>11</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="33">
         <v>3</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="16" t="s">
+      <c r="H14" s="33"/>
+      <c r="I14" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="14"/>
-      <c r="K14" s="13"/>
-      <c r="M14" s="32" t="s">
+      <c r="J14" s="33"/>
+      <c r="K14" s="5">
+        <v>106</v>
+      </c>
+      <c r="M14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="P14" s="33" t="s">
+      <c r="P14" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33" t="s">
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="S14" s="33"/>
-      <c r="T14" s="32" t="s">
+      <c r="S14" s="41"/>
+      <c r="T14" s="11" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F15" s="13">
+      <c r="F15" s="5">
         <v>12</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="33">
         <v>3</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="16" t="s">
+      <c r="H15" s="33"/>
+      <c r="I15" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="13"/>
-      <c r="M15" s="34">
+      <c r="J15" s="60"/>
+      <c r="K15" s="5">
+        <v>107</v>
+      </c>
+      <c r="M15" s="12">
         <v>1</v>
       </c>
-      <c r="N15" s="34">
+      <c r="N15" s="12">
         <v>3</v>
       </c>
-      <c r="O15" s="34" t="s">
+      <c r="O15" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="P15" s="35" t="s">
+      <c r="P15" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35">
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42">
         <v>2</v>
       </c>
-      <c r="S15" s="35"/>
-      <c r="T15" s="34">
+      <c r="S15" s="42"/>
+      <c r="T15" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="F16" s="18"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="18"/>
-      <c r="M16" s="34">
+      <c r="F16" s="7"/>
+      <c r="G16" s="49"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="7"/>
+      <c r="M16" s="12">
         <v>2</v>
       </c>
-      <c r="N16" s="34">
+      <c r="N16" s="12">
         <v>4</v>
       </c>
-      <c r="O16" s="34" t="s">
+      <c r="O16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="P16" s="35" t="s">
+      <c r="P16" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35">
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42">
         <v>17</v>
       </c>
-      <c r="S16" s="35"/>
-      <c r="T16" s="34">
+      <c r="S16" s="42"/>
+      <c r="T16" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="M17" s="34">
+      <c r="M17" s="12">
         <v>3</v>
       </c>
-      <c r="N17" s="34">
+      <c r="N17" s="12">
         <v>5</v>
       </c>
-      <c r="O17" s="34" t="s">
+      <c r="O17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P17" s="35" t="s">
+      <c r="P17" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35">
+      <c r="Q17" s="42"/>
+      <c r="R17" s="42">
         <v>16</v>
       </c>
-      <c r="S17" s="35"/>
-      <c r="T17" s="34">
+      <c r="S17" s="42"/>
+      <c r="T17" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1781,455 +1829,463 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="M20" s="36" t="s">
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="M20" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="36"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="36"/>
-      <c r="X20" s="36"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
+      <c r="X20" s="40"/>
     </row>
     <row r="21" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="43" t="s">
+      <c r="G21" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="M21" s="37" t="s">
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="M21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="38" t="s">
+      <c r="N21" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="O21" s="38"/>
-      <c r="P21" s="37" t="s">
+      <c r="O21" s="39"/>
+      <c r="P21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q21" s="38" t="s">
+      <c r="Q21" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="R21" s="38"/>
-      <c r="S21" s="38" t="s">
+      <c r="R21" s="39"/>
+      <c r="S21" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="T21" s="38"/>
-      <c r="U21" s="38" t="s">
+      <c r="T21" s="39"/>
+      <c r="U21" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="V21" s="38"/>
-      <c r="W21" s="38" t="s">
+      <c r="V21" s="39"/>
+      <c r="W21" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="X21" s="38"/>
+      <c r="X21" s="39"/>
     </row>
     <row r="22" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F22" s="46">
+      <c r="F22" s="16">
         <v>1</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="M22" s="39">
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="M22" s="14">
         <v>1</v>
       </c>
-      <c r="N22" s="40" t="s">
+      <c r="N22" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="O22" s="40"/>
-      <c r="P22" s="39">
+      <c r="O22" s="36"/>
+      <c r="P22" s="14">
         <v>532</v>
       </c>
-      <c r="Q22" s="40"/>
-      <c r="R22" s="40"/>
-      <c r="S22" s="40" t="s">
+      <c r="Q22" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="R22" s="36"/>
+      <c r="S22" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="T22" s="40"/>
-      <c r="U22" s="40" t="s">
+      <c r="T22" s="36"/>
+      <c r="U22" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="V22" s="40"/>
-      <c r="W22" s="40"/>
-      <c r="X22" s="40"/>
+      <c r="V22" s="36"/>
+      <c r="W22" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="X22" s="36"/>
     </row>
     <row r="23" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F23" s="46">
+      <c r="F23" s="16">
         <v>2</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G23" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="M23" s="39">
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="M23" s="14">
         <v>2</v>
       </c>
-      <c r="N23" s="40" t="s">
+      <c r="N23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="40"/>
-      <c r="P23" s="39">
+      <c r="O23" s="36"/>
+      <c r="P23" s="14">
         <v>240</v>
       </c>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="40"/>
-      <c r="S23" s="40" t="s">
+      <c r="Q23" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="R23" s="36"/>
+      <c r="S23" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="T23" s="40"/>
-      <c r="U23" s="40" t="s">
+      <c r="T23" s="36"/>
+      <c r="U23" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="V23" s="40"/>
-      <c r="W23" s="40" t="s">
+      <c r="V23" s="36"/>
+      <c r="W23" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="X23" s="40"/>
+      <c r="X23" s="36"/>
     </row>
     <row r="24" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F24" s="46">
+      <c r="F24" s="16">
         <v>3</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="M24" s="39">
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="M24" s="14">
         <v>3</v>
       </c>
-      <c r="N24" s="40" t="s">
+      <c r="N24" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="40"/>
-      <c r="P24" s="39">
+      <c r="O24" s="36"/>
+      <c r="P24" s="14">
         <v>1578</v>
       </c>
-      <c r="Q24" s="40" t="s">
+      <c r="Q24" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40" t="s">
+      <c r="R24" s="36"/>
+      <c r="S24" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40" t="s">
+      <c r="T24" s="36"/>
+      <c r="U24" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="V24" s="40"/>
-      <c r="W24" s="40" t="s">
+      <c r="V24" s="36"/>
+      <c r="W24" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="X24" s="40"/>
+      <c r="X24" s="36"/>
     </row>
     <row r="25" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F25" s="46">
+      <c r="F25" s="16">
         <v>4</v>
       </c>
-      <c r="G25" s="47" t="s">
+      <c r="G25" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="M25" s="39">
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="M25" s="14">
         <v>4</v>
       </c>
-      <c r="N25" s="40" t="s">
+      <c r="N25" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="O25" s="40"/>
-      <c r="P25" s="39">
+      <c r="O25" s="36"/>
+      <c r="P25" s="14">
         <v>2927</v>
       </c>
-      <c r="Q25" s="40" t="s">
+      <c r="Q25" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R25" s="40"/>
-      <c r="S25" s="40" t="s">
+      <c r="R25" s="36"/>
+      <c r="S25" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="T25" s="40"/>
-      <c r="U25" s="40" t="s">
+      <c r="T25" s="36"/>
+      <c r="U25" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="V25" s="40"/>
-      <c r="W25" s="40" t="s">
+      <c r="V25" s="36"/>
+      <c r="W25" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="X25" s="40"/>
+      <c r="X25" s="36"/>
     </row>
     <row r="26" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F26" s="46">
+      <c r="F26" s="16">
         <v>5</v>
       </c>
-      <c r="G26" s="47" t="s">
+      <c r="G26" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="M26" s="39">
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="M26" s="14">
         <v>5</v>
       </c>
-      <c r="N26" s="40" t="s">
+      <c r="N26" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="O26" s="40"/>
-      <c r="P26" s="39">
+      <c r="O26" s="36"/>
+      <c r="P26" s="14">
         <v>120</v>
       </c>
-      <c r="Q26" s="40" t="s">
+      <c r="Q26" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="R26" s="40"/>
-      <c r="S26" s="40" t="s">
+      <c r="R26" s="36"/>
+      <c r="S26" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="T26" s="40"/>
-      <c r="U26" s="40" t="s">
+      <c r="T26" s="36"/>
+      <c r="U26" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="V26" s="40"/>
-      <c r="W26" s="42" t="s">
+      <c r="V26" s="36"/>
+      <c r="W26" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="X26" s="42"/>
+      <c r="X26" s="37"/>
     </row>
     <row r="27" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F27" s="46">
+      <c r="F27" s="16">
         <v>6</v>
       </c>
-      <c r="G27" s="47" t="s">
+      <c r="G27" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
-      <c r="M27" s="39">
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="M27" s="14">
         <v>6</v>
       </c>
-      <c r="N27" s="40" t="s">
+      <c r="N27" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="O27" s="40"/>
-      <c r="P27" s="39">
+      <c r="O27" s="36"/>
+      <c r="P27" s="14">
         <v>66</v>
       </c>
-      <c r="Q27" s="40" t="s">
+      <c r="Q27" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="R27" s="40"/>
-      <c r="S27" s="40" t="s">
+      <c r="R27" s="36"/>
+      <c r="S27" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="T27" s="40"/>
-      <c r="U27" s="40" t="s">
+      <c r="T27" s="36"/>
+      <c r="U27" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="V27" s="40"/>
-      <c r="W27" s="42" t="s">
+      <c r="V27" s="36"/>
+      <c r="W27" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="X27" s="41"/>
+      <c r="X27" s="38"/>
     </row>
     <row r="28" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F28" s="46">
+      <c r="F28" s="16">
         <v>7</v>
       </c>
-      <c r="G28" s="47" t="s">
+      <c r="G28" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="M28" s="39">
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="M28" s="14">
         <v>7</v>
       </c>
-      <c r="N28" s="40" t="s">
+      <c r="N28" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="O28" s="40"/>
-      <c r="P28" s="39">
+      <c r="O28" s="36"/>
+      <c r="P28" s="14">
         <v>945</v>
       </c>
-      <c r="Q28" s="40" t="s">
+      <c r="Q28" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="R28" s="40"/>
-      <c r="S28" s="40" t="s">
+      <c r="R28" s="36"/>
+      <c r="S28" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="T28" s="40"/>
-      <c r="U28" s="40" t="s">
+      <c r="T28" s="36"/>
+      <c r="U28" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="V28" s="40"/>
-      <c r="W28" s="42" t="s">
+      <c r="V28" s="36"/>
+      <c r="W28" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="X28" s="42"/>
+      <c r="X28" s="37"/>
     </row>
     <row r="29" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F29" s="46">
+      <c r="F29" s="16">
         <v>8</v>
       </c>
-      <c r="G29" s="47" t="s">
+      <c r="G29" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="M29" s="39">
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="M29" s="14">
         <v>8</v>
       </c>
-      <c r="N29" s="40" t="s">
+      <c r="N29" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="O29" s="40"/>
-      <c r="P29" s="39">
+      <c r="O29" s="36"/>
+      <c r="P29" s="14">
         <v>232</v>
       </c>
-      <c r="Q29" s="40" t="s">
+      <c r="Q29" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="R29" s="40"/>
-      <c r="S29" s="40" t="s">
+      <c r="R29" s="36"/>
+      <c r="S29" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="T29" s="40"/>
-      <c r="U29" s="40" t="s">
+      <c r="T29" s="36"/>
+      <c r="U29" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="V29" s="40"/>
-      <c r="W29" s="40" t="s">
+      <c r="V29" s="36"/>
+      <c r="W29" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="X29" s="40"/>
+      <c r="X29" s="36"/>
     </row>
     <row r="30" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F30" s="46">
+      <c r="F30" s="16">
         <v>9</v>
       </c>
-      <c r="G30" s="47" t="s">
+      <c r="G30" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
     </row>
     <row r="31" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F31" s="46">
+      <c r="F31" s="16">
         <v>10</v>
       </c>
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
     </row>
     <row r="32" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F32" s="46">
+      <c r="F32" s="16">
         <v>11</v>
       </c>
-      <c r="G32" s="47" t="s">
+      <c r="G32" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="N32" s="54" t="s">
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="N32" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="O32" s="54"/>
-      <c r="P32" s="54"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="54"/>
-      <c r="S32" s="54"/>
-      <c r="T32" s="54"/>
-      <c r="U32" s="54"/>
-      <c r="V32" s="54"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="21"/>
+      <c r="V32" s="21"/>
     </row>
     <row r="33" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F33" s="46">
+      <c r="F33" s="16">
         <v>12</v>
       </c>
-      <c r="G33" s="47" t="s">
+      <c r="G33" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="47"/>
-      <c r="I33" s="47"/>
-      <c r="N33" s="55" t="s">
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="N33" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="O33" s="55" t="s">
+      <c r="O33" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P33" s="55" t="s">
+      <c r="P33" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="Q33" s="56" t="s">
+      <c r="Q33" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="R33" s="56"/>
-      <c r="S33" s="56" t="s">
+      <c r="R33" s="19"/>
+      <c r="S33" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="T33" s="56"/>
-      <c r="U33" s="56" t="s">
+      <c r="T33" s="19"/>
+      <c r="U33" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="V33" s="56"/>
+      <c r="V33" s="19"/>
     </row>
     <row r="34" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F34" s="46">
+      <c r="F34" s="16">
         <v>13</v>
       </c>
-      <c r="G34" s="47" t="s">
+      <c r="G34" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="N34" s="57">
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="N34" s="18">
         <v>1</v>
       </c>
-      <c r="O34" s="57">
+      <c r="O34" s="18">
         <v>1</v>
       </c>
-      <c r="P34" s="57"/>
-      <c r="Q34" s="58" t="s">
+      <c r="P34" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q34" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58" t="s">
+      <c r="R34" s="20"/>
+      <c r="S34" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="T34" s="58"/>
-      <c r="U34" s="58" t="s">
+      <c r="T34" s="20"/>
+      <c r="U34" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="V34" s="58"/>
+      <c r="V34" s="20"/>
     </row>
     <row r="35" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F35" s="46">
+      <c r="F35" s="16">
         <v>14</v>
       </c>
-      <c r="G35" s="47" t="s">
+      <c r="G35" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -2238,14 +2294,14 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F36" s="46">
+      <c r="F36" s="16">
         <v>15</v>
       </c>
-      <c r="G36" s="47" t="s">
+      <c r="G36" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -2254,14 +2310,14 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F37" s="46">
+      <c r="F37" s="16">
         <v>16</v>
       </c>
-      <c r="G37" s="48" t="s">
+      <c r="G37" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="28"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -2270,14 +2326,14 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F38" s="46">
+      <c r="F38" s="16">
         <v>17</v>
       </c>
-      <c r="G38" s="48" t="s">
+      <c r="G38" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="50"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="28"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -2286,181 +2342,181 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
-      <c r="I39" s="18"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
     </row>
     <row r="41" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10"/>
-      <c r="L41" s="10"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
     </row>
     <row r="42" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="12" t="s">
+      <c r="G42" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="12"/>
-      <c r="I42" s="11" t="s">
+      <c r="H42" s="24"/>
+      <c r="I42" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="J42" s="11" t="s">
+      <c r="J42" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="K42" s="12" t="s">
+      <c r="K42" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="L42" s="12"/>
+      <c r="L42" s="61"/>
     </row>
     <row r="43" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F43" s="13">
+      <c r="F43" s="5">
         <v>1</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="33">
         <v>7</v>
       </c>
-      <c r="H43" s="14"/>
-      <c r="I43" s="13">
+      <c r="H43" s="33"/>
+      <c r="I43" s="5">
         <v>3</v>
       </c>
-      <c r="J43" s="13">
+      <c r="J43" s="5">
         <v>1</v>
       </c>
-      <c r="K43" s="51">
+      <c r="K43" s="32">
         <v>43850.625</v>
       </c>
-      <c r="L43" s="14"/>
+      <c r="L43" s="33"/>
     </row>
     <row r="44" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F44" s="13">
+      <c r="F44" s="5">
         <v>2</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="33">
         <v>2</v>
       </c>
-      <c r="H44" s="14"/>
-      <c r="I44" s="13">
+      <c r="H44" s="33"/>
+      <c r="I44" s="5">
         <v>2</v>
       </c>
-      <c r="J44" s="13">
+      <c r="J44" s="5">
         <v>3</v>
       </c>
-      <c r="K44" s="51">
+      <c r="K44" s="32">
         <v>43836.416666666664</v>
       </c>
-      <c r="L44" s="14"/>
+      <c r="L44" s="33"/>
     </row>
     <row r="45" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F45" s="13">
+      <c r="F45" s="5">
         <v>3</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="33">
         <v>3</v>
       </c>
-      <c r="H45" s="14"/>
-      <c r="I45" s="13">
+      <c r="H45" s="33"/>
+      <c r="I45" s="5">
         <v>2</v>
       </c>
-      <c r="J45" s="13">
+      <c r="J45" s="5">
         <v>1</v>
       </c>
-      <c r="K45" s="51">
+      <c r="K45" s="32">
         <v>43868.458333333336</v>
       </c>
-      <c r="L45" s="14"/>
+      <c r="L45" s="33"/>
     </row>
     <row r="46" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F46" s="13">
+      <c r="F46" s="5">
         <v>4</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="33">
         <v>2</v>
       </c>
-      <c r="H46" s="14"/>
-      <c r="I46" s="13">
+      <c r="H46" s="33"/>
+      <c r="I46" s="5">
         <v>2</v>
       </c>
-      <c r="J46" s="13">
+      <c r="J46" s="5">
         <v>1</v>
       </c>
-      <c r="K46" s="51">
+      <c r="K46" s="32">
         <v>43137.416666666664</v>
       </c>
-      <c r="L46" s="14"/>
+      <c r="L46" s="33"/>
     </row>
     <row r="47" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F47" s="13">
+      <c r="F47" s="5">
         <v>5</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="33">
         <v>4</v>
       </c>
-      <c r="H47" s="14"/>
-      <c r="I47" s="13">
+      <c r="H47" s="33"/>
+      <c r="I47" s="5">
         <v>1</v>
       </c>
-      <c r="J47" s="13">
+      <c r="J47" s="5">
         <v>3</v>
       </c>
-      <c r="K47" s="51">
+      <c r="K47" s="32">
         <v>43503.458854166667</v>
       </c>
-      <c r="L47" s="14"/>
+      <c r="L47" s="33"/>
     </row>
     <row r="48" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F48" s="13">
+      <c r="F48" s="5">
         <v>6</v>
       </c>
-      <c r="G48" s="14">
+      <c r="G48" s="33">
         <v>7</v>
       </c>
-      <c r="H48" s="14"/>
-      <c r="I48" s="13">
+      <c r="H48" s="33"/>
+      <c r="I48" s="5">
         <v>3</v>
       </c>
-      <c r="J48" s="13">
+      <c r="J48" s="5">
         <v>2</v>
       </c>
-      <c r="K48" s="51">
+      <c r="K48" s="32">
         <v>43898.625</v>
       </c>
-      <c r="L48" s="14"/>
+      <c r="L48" s="33"/>
     </row>
     <row r="49" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F49" s="13">
+      <c r="F49" s="5">
         <v>7</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="33">
         <v>4</v>
       </c>
-      <c r="H49" s="14"/>
-      <c r="I49" s="13">
+      <c r="H49" s="33"/>
+      <c r="I49" s="5">
         <v>1</v>
       </c>
-      <c r="J49" s="13">
+      <c r="J49" s="5">
         <v>2</v>
       </c>
-      <c r="K49" s="51">
+      <c r="K49" s="32">
         <v>43899.458854166667</v>
       </c>
-      <c r="L49" s="14"/>
+      <c r="L49" s="33"/>
     </row>
     <row r="53" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F53" s="52" t="s">
+      <c r="F53" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="G53" s="52"/>
-      <c r="H53" s="52"/>
-      <c r="I53" s="30"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="10"/>
       <c r="J53" t="s">
         <v>119</v>
       </c>
@@ -2469,22 +2525,22 @@
       </c>
     </row>
     <row r="54" spans="6:14" x14ac:dyDescent="0.25">
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G54" s="53" t="s">
+      <c r="G54" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="H54" s="53"/>
+      <c r="H54" s="22"/>
     </row>
     <row r="55" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F55" s="2">
         <v>1</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="G55" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="H55" s="6"/>
+      <c r="H55" s="31"/>
       <c r="K55" t="s">
         <v>118</v>
       </c>
@@ -2499,10 +2555,10 @@
       <c r="F56" s="2">
         <v>2</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="G56" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="H56" s="6"/>
+      <c r="H56" s="31"/>
       <c r="L56" t="s">
         <v>116</v>
       </c>
@@ -2514,10 +2570,10 @@
       <c r="F57" s="2">
         <v>3</v>
       </c>
-      <c r="G57" s="5" t="s">
+      <c r="G57" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="H57" s="6"/>
+      <c r="H57" s="31"/>
       <c r="M57" t="s">
         <v>115</v>
       </c>
@@ -2529,125 +2585,37 @@
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="N32:V32"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="F41:L41"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="W29:X29"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="M20:X20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="M13:T13"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
@@ -2668,37 +2636,125 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="M13:T13"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="M20:X20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="W29:X29"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="N32:V32"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="F41:L41"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{7413389C-42AD-4264-AF93-E4F1B4F7BAC2}"/>
@@ -2710,9 +2766,9 @@
     <hyperlink ref="I12" r:id="rId7" xr:uid="{104FDB43-A8DC-426A-91B9-6E4320A3D63D}"/>
     <hyperlink ref="I13" r:id="rId8" xr:uid="{CD88C040-7DED-412A-BE5A-C9EB791958B9}"/>
     <hyperlink ref="I14" r:id="rId9" xr:uid="{4407F112-A0BA-47A2-9B14-6445460E31D1}"/>
-    <hyperlink ref="I15" r:id="rId10" xr:uid="{6B92B389-AED6-49B4-9CD2-CAECEC78E17B}"/>
-    <hyperlink ref="I7" r:id="rId11" xr:uid="{3E761C81-56E4-47CB-A9E9-09EF163B4CDF}"/>
-    <hyperlink ref="I8" r:id="rId12" xr:uid="{481E7917-B929-418C-81D9-359F118EB6D8}"/>
+    <hyperlink ref="I7" r:id="rId10" xr:uid="{3E761C81-56E4-47CB-A9E9-09EF163B4CDF}"/>
+    <hyperlink ref="I8" r:id="rId11" xr:uid="{481E7917-B929-418C-81D9-359F118EB6D8}"/>
+    <hyperlink ref="I15" r:id="rId12" xr:uid="{6B92B389-AED6-49B4-9CD2-CAECEC78E17B}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Modelagens Finalizadascom Fisico SSMS
</commit_message>
<xml_diff>
--- a/Modelagens/Modelagens_SpMedGroup-Físico.xlsx
+++ b/Modelagens/Modelagens_SpMedGroup-Físico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livia\OneDrive\Documents\Lívia\Lívia Escola\SENAI\sprint-1-bd\exercicios\SpMedGroup\Modelagens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D473028-5FFA-419B-BD27-4DF2F1E8E381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2ED8A8B4-C7D3-4A50-899E-8BA3C14123AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{03839324-049D-4BCD-8CB4-4926F755280E}"/>
   </bookViews>
@@ -745,167 +745,167 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="23" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1233,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CE33BF-5118-4F54-98F8-364B9B925BD9}">
   <dimension ref="B2:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
@@ -1255,53 +1255,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="F2" s="27" t="s">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="F2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="M2" s="36" t="s">
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="M2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="38"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="71"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="76"/>
       <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="42"/>
+      <c r="I3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="42"/>
       <c r="K3" s="4" t="s">
         <v>8</v>
       </c>
@@ -1318,42 +1318,42 @@
       <c r="P3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="Q3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="29"/>
-      <c r="S3" s="28" t="s">
+      <c r="R3" s="68"/>
+      <c r="S3" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="29"/>
-      <c r="U3" s="28" t="s">
+      <c r="T3" s="68"/>
+      <c r="U3" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="29"/>
-      <c r="W3" s="28" t="s">
+      <c r="V3" s="68"/>
+      <c r="W3" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="29"/>
+      <c r="X3" s="68"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="73"/>
       <c r="F4" s="5">
         <v>1</v>
       </c>
-      <c r="G4" s="26">
+      <c r="G4" s="48">
         <v>1</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="25" t="s">
+      <c r="H4" s="48"/>
+      <c r="I4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="26"/>
+      <c r="J4" s="48"/>
       <c r="K4" s="5">
         <v>123</v>
       </c>
@@ -1369,42 +1369,42 @@
       <c r="P4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="30">
+      <c r="Q4" s="58">
         <v>30602</v>
       </c>
-      <c r="R4" s="31"/>
-      <c r="S4" s="34" t="s">
+      <c r="R4" s="59"/>
+      <c r="S4" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="35"/>
-      <c r="U4" s="34">
+      <c r="T4" s="62"/>
+      <c r="U4" s="61">
         <v>432124576</v>
       </c>
-      <c r="V4" s="35"/>
-      <c r="W4" s="34">
+      <c r="V4" s="62"/>
+      <c r="W4" s="61">
         <v>94839859000</v>
       </c>
-      <c r="X4" s="35"/>
+      <c r="X4" s="62"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="73"/>
       <c r="F5" s="5">
         <v>2</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="48">
         <v>1</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="25" t="s">
+      <c r="H5" s="48"/>
+      <c r="I5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="26"/>
+      <c r="J5" s="48"/>
       <c r="K5" s="5">
         <v>345</v>
       </c>
@@ -1420,42 +1420,42 @@
       <c r="P5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="58">
         <v>37095</v>
       </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="34" t="s">
+      <c r="R5" s="59"/>
+      <c r="S5" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="35"/>
-      <c r="U5" s="34" t="s">
+      <c r="T5" s="62"/>
+      <c r="U5" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="35"/>
-      <c r="W5" s="34">
+      <c r="V5" s="62"/>
+      <c r="W5" s="61">
         <v>73556944057</v>
       </c>
-      <c r="X5" s="35"/>
+      <c r="X5" s="62"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="73"/>
       <c r="F6" s="5">
         <v>3</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="48">
         <v>2</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="25" t="s">
+      <c r="H6" s="48"/>
+      <c r="I6" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="26"/>
+      <c r="J6" s="48"/>
       <c r="K6" s="5">
         <v>567</v>
       </c>
@@ -1471,35 +1471,35 @@
       <c r="P6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="58">
         <v>28773</v>
       </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="34" t="s">
+      <c r="R6" s="59"/>
+      <c r="S6" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="T6" s="35"/>
-      <c r="U6" s="34" t="s">
+      <c r="T6" s="62"/>
+      <c r="U6" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="V6" s="35"/>
-      <c r="W6" s="34">
+      <c r="V6" s="62"/>
+      <c r="W6" s="61">
         <v>16839338002</v>
       </c>
-      <c r="X6" s="35"/>
+      <c r="X6" s="62"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F7" s="5">
         <v>4</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="48">
         <v>2</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="25" t="s">
+      <c r="H7" s="48"/>
+      <c r="I7" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="48"/>
       <c r="K7" s="5">
         <v>789</v>
       </c>
@@ -1515,35 +1515,35 @@
       <c r="P7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" s="30">
+      <c r="Q7" s="58">
         <v>31333</v>
       </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="34" t="s">
+      <c r="R7" s="59"/>
+      <c r="S7" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="35"/>
-      <c r="U7" s="34" t="s">
+      <c r="T7" s="62"/>
+      <c r="U7" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="V7" s="35"/>
-      <c r="W7" s="34">
+      <c r="V7" s="62"/>
+      <c r="W7" s="61">
         <v>14332654765</v>
       </c>
-      <c r="X7" s="35"/>
+      <c r="X7" s="62"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F8" s="5">
         <v>5</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="48">
         <v>2</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="25" t="s">
+      <c r="H8" s="48"/>
+      <c r="I8" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="J8" s="26"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="5">
         <v>910</v>
       </c>
@@ -1559,35 +1559,35 @@
       <c r="P8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="Q8" s="58">
         <v>27633</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="34" t="s">
+      <c r="R8" s="59"/>
+      <c r="S8" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="T8" s="35"/>
-      <c r="U8" s="34" t="s">
+      <c r="T8" s="62"/>
+      <c r="U8" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="V8" s="35"/>
-      <c r="W8" s="34">
+      <c r="V8" s="62"/>
+      <c r="W8" s="61">
         <v>91305348010</v>
       </c>
-      <c r="X8" s="35"/>
+      <c r="X8" s="62"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F9" s="5">
         <v>6</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="48">
         <v>3</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="25" t="s">
+      <c r="H9" s="48"/>
+      <c r="I9" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="26"/>
+      <c r="J9" s="48"/>
       <c r="K9" s="5">
         <v>101</v>
       </c>
@@ -1603,35 +1603,35 @@
       <c r="P9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="Q9" s="58">
         <v>26379</v>
       </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="34" t="s">
+      <c r="R9" s="59"/>
+      <c r="S9" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="T9" s="35"/>
-      <c r="U9" s="34" t="s">
+      <c r="T9" s="62"/>
+      <c r="U9" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="V9" s="35"/>
-      <c r="W9" s="34">
+      <c r="V9" s="62"/>
+      <c r="W9" s="61">
         <v>79799299004</v>
       </c>
-      <c r="X9" s="35"/>
+      <c r="X9" s="62"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F10" s="5">
         <v>7</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="48">
         <v>3</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="25" t="s">
+      <c r="H10" s="48"/>
+      <c r="I10" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="26"/>
+      <c r="J10" s="48"/>
       <c r="K10" s="5">
         <v>102</v>
       </c>
@@ -1647,33 +1647,33 @@
       <c r="P10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="30">
+      <c r="Q10" s="58">
         <v>43164</v>
       </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="34" t="s">
+      <c r="R10" s="59"/>
+      <c r="S10" s="61"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="V10" s="35"/>
-      <c r="W10" s="34">
+      <c r="V10" s="62"/>
+      <c r="W10" s="61">
         <v>13771913039</v>
       </c>
-      <c r="X10" s="35"/>
+      <c r="X10" s="62"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F11" s="5">
         <v>8</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="48">
         <v>3</v>
       </c>
-      <c r="H11" s="26"/>
-      <c r="I11" s="25" t="s">
+      <c r="H11" s="48"/>
+      <c r="I11" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="26"/>
+      <c r="J11" s="48"/>
       <c r="K11" s="5">
         <v>103</v>
       </c>
@@ -1694,14 +1694,14 @@
       <c r="F12" s="5">
         <v>9</v>
       </c>
-      <c r="G12" s="26">
+      <c r="G12" s="48">
         <v>3</v>
       </c>
-      <c r="H12" s="26"/>
-      <c r="I12" s="25" t="s">
+      <c r="H12" s="48"/>
+      <c r="I12" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J12" s="48"/>
       <c r="K12" s="5">
         <v>104</v>
       </c>
@@ -1710,40 +1710,40 @@
       <c r="F13" s="5">
         <v>10</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="48">
         <v>3</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="25" t="s">
+      <c r="H13" s="48"/>
+      <c r="I13" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="26"/>
+      <c r="J13" s="48"/>
       <c r="K13" s="5">
         <v>105</v>
       </c>
-      <c r="M13" s="42" t="s">
+      <c r="M13" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F14" s="5">
         <v>11</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="48">
         <v>3</v>
       </c>
-      <c r="H14" s="26"/>
-      <c r="I14" s="25" t="s">
+      <c r="H14" s="48"/>
+      <c r="I14" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="26"/>
+      <c r="J14" s="48"/>
       <c r="K14" s="5">
         <v>106</v>
       </c>
@@ -1756,14 +1756,14 @@
       <c r="O14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="P14" s="43" t="s">
+      <c r="P14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="43" t="s">
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="S14" s="43"/>
+      <c r="S14" s="56"/>
       <c r="T14" s="11" t="s">
         <v>49</v>
       </c>
@@ -1772,14 +1772,14 @@
       <c r="F15" s="5">
         <v>12</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="48">
         <v>3</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="40" t="s">
+      <c r="H15" s="48"/>
+      <c r="I15" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="41"/>
+      <c r="J15" s="66"/>
       <c r="K15" s="5">
         <v>107</v>
       </c>
@@ -1792,24 +1792,24 @@
       <c r="O15" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="P15" s="44" t="s">
+      <c r="P15" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44">
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57">
         <v>2</v>
       </c>
-      <c r="S15" s="44"/>
+      <c r="S15" s="57"/>
       <c r="T15" s="12">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F16" s="7"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
       <c r="K16" s="7"/>
       <c r="M16" s="12">
         <v>2</v>
@@ -1820,14 +1820,14 @@
       <c r="O16" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="P16" s="44" t="s">
+      <c r="P16" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44">
+      <c r="Q16" s="57"/>
+      <c r="R16" s="57">
         <v>17</v>
       </c>
-      <c r="S16" s="44"/>
+      <c r="S16" s="57"/>
       <c r="T16" s="12">
         <v>1</v>
       </c>
@@ -1842,14 +1842,14 @@
       <c r="O17" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="P17" s="44" t="s">
+      <c r="P17" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44">
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57">
         <v>16</v>
       </c>
-      <c r="S17" s="44"/>
+      <c r="S17" s="57"/>
       <c r="T17" s="12">
         <v>1</v>
       </c>
@@ -1873,402 +1873,402 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="6:24" x14ac:dyDescent="0.25">
-      <c r="F20" s="52" t="s">
+      <c r="F20" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="M20" s="47" t="s">
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="M20" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="47"/>
-      <c r="U20" s="47"/>
-      <c r="V20" s="47"/>
-      <c r="W20" s="47"/>
-      <c r="X20" s="47"/>
+      <c r="N20" s="55"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="55"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
     </row>
     <row r="21" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G21" s="51" t="s">
+      <c r="G21" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
       <c r="M21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N21" s="46" t="s">
+      <c r="N21" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="O21" s="46"/>
+      <c r="O21" s="54"/>
       <c r="P21" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q21" s="46" t="s">
+      <c r="Q21" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="R21" s="46"/>
-      <c r="S21" s="46" t="s">
+      <c r="R21" s="54"/>
+      <c r="S21" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="T21" s="46"/>
-      <c r="U21" s="46" t="s">
+      <c r="T21" s="54"/>
+      <c r="U21" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="V21" s="46"/>
-      <c r="W21" s="46" t="s">
+      <c r="V21" s="54"/>
+      <c r="W21" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="X21" s="46"/>
+      <c r="X21" s="54"/>
     </row>
     <row r="22" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F22" s="16">
         <v>1</v>
       </c>
-      <c r="G22" s="50" t="s">
+      <c r="G22" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
       <c r="M22" s="14">
         <v>1</v>
       </c>
-      <c r="N22" s="45" t="s">
+      <c r="N22" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="O22" s="45"/>
+      <c r="O22" s="51"/>
       <c r="P22" s="14">
         <v>532</v>
       </c>
-      <c r="Q22" s="45" t="s">
+      <c r="Q22" s="51" t="s">
         <v>131</v>
       </c>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45" t="s">
+      <c r="R22" s="51"/>
+      <c r="S22" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="T22" s="45"/>
-      <c r="U22" s="45" t="s">
+      <c r="T22" s="51"/>
+      <c r="U22" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="V22" s="45"/>
-      <c r="W22" s="45" t="s">
+      <c r="V22" s="51"/>
+      <c r="W22" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="X22" s="45"/>
+      <c r="X22" s="51"/>
     </row>
     <row r="23" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F23" s="16">
         <v>2</v>
       </c>
-      <c r="G23" s="50" t="s">
+      <c r="G23" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
       <c r="M23" s="14">
         <v>2</v>
       </c>
-      <c r="N23" s="45" t="s">
+      <c r="N23" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="O23" s="45"/>
+      <c r="O23" s="51"/>
       <c r="P23" s="14">
         <v>240</v>
       </c>
-      <c r="Q23" s="45" t="s">
+      <c r="Q23" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45" t="s">
+      <c r="R23" s="51"/>
+      <c r="S23" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="T23" s="45"/>
-      <c r="U23" s="45" t="s">
+      <c r="T23" s="51"/>
+      <c r="U23" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="V23" s="45"/>
-      <c r="W23" s="45" t="s">
+      <c r="V23" s="51"/>
+      <c r="W23" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="X23" s="45"/>
+      <c r="X23" s="51"/>
     </row>
     <row r="24" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F24" s="16">
         <v>3</v>
       </c>
-      <c r="G24" s="50" t="s">
+      <c r="G24" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="50"/>
-      <c r="I24" s="50"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
       <c r="M24" s="14">
         <v>3</v>
       </c>
-      <c r="N24" s="45" t="s">
+      <c r="N24" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="45"/>
+      <c r="O24" s="51"/>
       <c r="P24" s="14">
         <v>1578</v>
       </c>
-      <c r="Q24" s="45" t="s">
+      <c r="Q24" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="R24" s="45"/>
-      <c r="S24" s="45" t="s">
+      <c r="R24" s="51"/>
+      <c r="S24" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="T24" s="45"/>
-      <c r="U24" s="45" t="s">
+      <c r="T24" s="51"/>
+      <c r="U24" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="V24" s="45"/>
-      <c r="W24" s="45" t="s">
+      <c r="V24" s="51"/>
+      <c r="W24" s="51" t="s">
         <v>71</v>
       </c>
-      <c r="X24" s="45"/>
+      <c r="X24" s="51"/>
     </row>
     <row r="25" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F25" s="16">
         <v>4</v>
       </c>
-      <c r="G25" s="50" t="s">
+      <c r="G25" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="50"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
       <c r="M25" s="14">
         <v>4</v>
       </c>
-      <c r="N25" s="45" t="s">
+      <c r="N25" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="O25" s="45"/>
+      <c r="O25" s="51"/>
       <c r="P25" s="14">
         <v>2927</v>
       </c>
-      <c r="Q25" s="45" t="s">
+      <c r="Q25" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45" t="s">
+      <c r="R25" s="51"/>
+      <c r="S25" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45" t="s">
+      <c r="T25" s="51"/>
+      <c r="U25" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="V25" s="45"/>
-      <c r="W25" s="45" t="s">
+      <c r="V25" s="51"/>
+      <c r="W25" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="X25" s="45"/>
+      <c r="X25" s="51"/>
     </row>
     <row r="26" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F26" s="16">
         <v>5</v>
       </c>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
       <c r="M26" s="14">
         <v>5</v>
       </c>
-      <c r="N26" s="45" t="s">
+      <c r="N26" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="O26" s="45"/>
+      <c r="O26" s="51"/>
       <c r="P26" s="14">
         <v>120</v>
       </c>
-      <c r="Q26" s="45" t="s">
+      <c r="Q26" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45" t="s">
+      <c r="R26" s="51"/>
+      <c r="S26" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45" t="s">
+      <c r="T26" s="51"/>
+      <c r="U26" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="V26" s="45"/>
-      <c r="W26" s="48" t="s">
+      <c r="V26" s="51"/>
+      <c r="W26" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="X26" s="48"/>
+      <c r="X26" s="52"/>
     </row>
     <row r="27" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F27" s="16">
         <v>6</v>
       </c>
-      <c r="G27" s="50" t="s">
+      <c r="G27" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
       <c r="M27" s="14">
         <v>6</v>
       </c>
-      <c r="N27" s="45" t="s">
+      <c r="N27" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="O27" s="45"/>
+      <c r="O27" s="51"/>
       <c r="P27" s="14">
         <v>66</v>
       </c>
-      <c r="Q27" s="45" t="s">
+      <c r="Q27" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45" t="s">
+      <c r="R27" s="51"/>
+      <c r="S27" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45" t="s">
+      <c r="T27" s="51"/>
+      <c r="U27" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="V27" s="45"/>
-      <c r="W27" s="48" t="s">
+      <c r="V27" s="51"/>
+      <c r="W27" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="X27" s="49"/>
+      <c r="X27" s="53"/>
     </row>
     <row r="28" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F28" s="16">
         <v>7</v>
       </c>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
       <c r="M28" s="14">
         <v>7</v>
       </c>
-      <c r="N28" s="45" t="s">
+      <c r="N28" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="O28" s="45"/>
+      <c r="O28" s="51"/>
       <c r="P28" s="14">
         <v>945</v>
       </c>
-      <c r="Q28" s="45" t="s">
+      <c r="Q28" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45" t="s">
+      <c r="R28" s="51"/>
+      <c r="S28" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45" t="s">
+      <c r="T28" s="51"/>
+      <c r="U28" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="V28" s="45"/>
-      <c r="W28" s="48" t="s">
+      <c r="V28" s="51"/>
+      <c r="W28" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="X28" s="48"/>
+      <c r="X28" s="52"/>
     </row>
     <row r="29" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F29" s="16">
         <v>8</v>
       </c>
-      <c r="G29" s="50" t="s">
+      <c r="G29" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
       <c r="M29" s="14">
         <v>8</v>
       </c>
-      <c r="N29" s="45" t="s">
+      <c r="N29" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="O29" s="45"/>
+      <c r="O29" s="51"/>
       <c r="P29" s="14">
         <v>232</v>
       </c>
-      <c r="Q29" s="45" t="s">
+      <c r="Q29" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45" t="s">
+      <c r="R29" s="51"/>
+      <c r="S29" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45" t="s">
+      <c r="T29" s="51"/>
+      <c r="U29" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="V29" s="45"/>
-      <c r="W29" s="45" t="s">
+      <c r="V29" s="51"/>
+      <c r="W29" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="X29" s="45"/>
+      <c r="X29" s="51"/>
     </row>
     <row r="30" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F30" s="16">
         <v>9</v>
       </c>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
     </row>
     <row r="31" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F31" s="16">
         <v>10</v>
       </c>
-      <c r="G31" s="50" t="s">
+      <c r="G31" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
     </row>
     <row r="32" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F32" s="16">
         <v>11</v>
       </c>
-      <c r="G32" s="50" t="s">
+      <c r="G32" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="M32" s="61" t="s">
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="M32" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="N32" s="62"/>
-      <c r="O32" s="62"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
-      <c r="R32" s="62"/>
-      <c r="S32" s="62"/>
-      <c r="T32" s="62"/>
-      <c r="U32" s="62"/>
-      <c r="V32" s="63"/>
+      <c r="N32" s="44"/>
+      <c r="O32" s="44"/>
+      <c r="P32" s="44"/>
+      <c r="Q32" s="44"/>
+      <c r="R32" s="44"/>
+      <c r="S32" s="44"/>
+      <c r="T32" s="44"/>
+      <c r="U32" s="44"/>
+      <c r="V32" s="45"/>
     </row>
     <row r="33" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F33" s="16">
         <v>12</v>
       </c>
-      <c r="G33" s="50" t="s">
+      <c r="G33" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
       <c r="M33" s="17" t="s">
         <v>49</v>
       </c>
@@ -2281,62 +2281,62 @@
       <c r="P33" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="Q33" s="64" t="s">
+      <c r="Q33" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="R33" s="65"/>
-      <c r="S33" s="64" t="s">
+      <c r="R33" s="31"/>
+      <c r="S33" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="T33" s="65"/>
-      <c r="U33" s="64" t="s">
+      <c r="T33" s="31"/>
+      <c r="U33" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="V33" s="65"/>
+      <c r="V33" s="31"/>
     </row>
     <row r="34" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F34" s="16">
         <v>13</v>
       </c>
-      <c r="G34" s="50" t="s">
+      <c r="G34" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
       <c r="M34" s="18">
         <v>1</v>
       </c>
       <c r="N34" s="18">
         <v>1</v>
       </c>
-      <c r="O34" s="60">
+      <c r="O34" s="22">
         <v>0.33333333333333331</v>
       </c>
       <c r="P34" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="Q34" s="66" t="s">
+      <c r="Q34" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="R34" s="67"/>
-      <c r="S34" s="66" t="s">
+      <c r="R34" s="33"/>
+      <c r="S34" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="T34" s="67"/>
-      <c r="U34" s="66" t="s">
+      <c r="T34" s="33"/>
+      <c r="U34" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="V34" s="67"/>
+      <c r="V34" s="33"/>
     </row>
     <row r="35" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F35" s="16">
         <v>14</v>
       </c>
-      <c r="G35" s="50" t="s">
+      <c r="G35" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
@@ -2348,11 +2348,11 @@
       <c r="F36" s="16">
         <v>15</v>
       </c>
-      <c r="G36" s="50" t="s">
+      <c r="G36" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -2364,11 +2364,11 @@
       <c r="F37" s="16">
         <v>16</v>
       </c>
-      <c r="G37" s="57" t="s">
+      <c r="G37" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="H37" s="58"/>
-      <c r="I37" s="59"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -2380,11 +2380,11 @@
       <c r="F38" s="16">
         <v>17</v>
       </c>
-      <c r="G38" s="57" t="s">
+      <c r="G38" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="H38" s="58"/>
-      <c r="I38" s="59"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="41"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -2397,263 +2397,263 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
-      <c r="N39" s="70"/>
-      <c r="O39" s="70"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
     </row>
     <row r="40" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="N40" s="70"/>
-      <c r="O40" s="70"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
     </row>
     <row r="41" spans="6:22" x14ac:dyDescent="0.25">
-      <c r="F41" s="74" t="s">
+      <c r="F41" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="76"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="28"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+      <c r="L41" s="28"/>
+      <c r="M41" s="29"/>
       <c r="N41" s="6"/>
-      <c r="O41" s="70"/>
+      <c r="O41" s="23"/>
     </row>
     <row r="42" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F42" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="24"/>
+      <c r="H42" s="42"/>
       <c r="I42" s="19" t="s">
         <v>110</v>
       </c>
       <c r="J42" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="K42" s="68" t="s">
+      <c r="K42" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="L42" s="69"/>
+      <c r="L42" s="37"/>
       <c r="M42" s="19" t="s">
         <v>136</v>
       </c>
       <c r="N42" s="6"/>
-      <c r="O42" s="70"/>
+      <c r="O42" s="23"/>
     </row>
     <row r="43" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F43" s="21">
         <v>1</v>
       </c>
-      <c r="G43" s="26">
+      <c r="G43" s="48">
         <v>7</v>
       </c>
-      <c r="H43" s="26"/>
+      <c r="H43" s="48"/>
       <c r="I43" s="21">
         <v>3</v>
       </c>
       <c r="J43" s="21">
         <v>1</v>
       </c>
-      <c r="K43" s="71">
+      <c r="K43" s="25">
         <v>43850</v>
       </c>
-      <c r="L43" s="72"/>
+      <c r="L43" s="26"/>
       <c r="M43" s="20" t="s">
         <v>137</v>
       </c>
       <c r="N43" s="6"/>
-      <c r="O43" s="70"/>
+      <c r="O43" s="23"/>
     </row>
     <row r="44" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F44" s="21">
         <v>2</v>
       </c>
-      <c r="G44" s="26">
+      <c r="G44" s="48">
         <v>2</v>
       </c>
-      <c r="H44" s="26"/>
+      <c r="H44" s="48"/>
       <c r="I44" s="21">
         <v>2</v>
       </c>
       <c r="J44" s="21">
         <v>3</v>
       </c>
-      <c r="K44" s="71">
+      <c r="K44" s="25">
         <v>43836</v>
       </c>
-      <c r="L44" s="72"/>
-      <c r="M44" s="73">
+      <c r="L44" s="26"/>
+      <c r="M44" s="24">
         <v>0.41666666666666669</v>
       </c>
       <c r="N44" s="6"/>
-      <c r="O44" s="70"/>
+      <c r="O44" s="23"/>
     </row>
     <row r="45" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F45" s="21">
         <v>3</v>
       </c>
-      <c r="G45" s="26">
+      <c r="G45" s="48">
         <v>3</v>
       </c>
-      <c r="H45" s="26"/>
+      <c r="H45" s="48"/>
       <c r="I45" s="21">
         <v>2</v>
       </c>
       <c r="J45" s="21">
         <v>1</v>
       </c>
-      <c r="K45" s="71">
+      <c r="K45" s="25">
         <v>43868</v>
       </c>
-      <c r="L45" s="72"/>
-      <c r="M45" s="73">
+      <c r="L45" s="26"/>
+      <c r="M45" s="24">
         <v>0.45833333333333331</v>
       </c>
       <c r="N45" s="6"/>
-      <c r="O45" s="70"/>
+      <c r="O45" s="23"/>
     </row>
     <row r="46" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F46" s="21">
         <v>4</v>
       </c>
-      <c r="G46" s="26">
+      <c r="G46" s="48">
         <v>2</v>
       </c>
-      <c r="H46" s="26"/>
+      <c r="H46" s="48"/>
       <c r="I46" s="21">
         <v>2</v>
       </c>
       <c r="J46" s="21">
         <v>1</v>
       </c>
-      <c r="K46" s="71">
+      <c r="K46" s="25">
         <v>43137</v>
       </c>
-      <c r="L46" s="72"/>
-      <c r="M46" s="73">
+      <c r="L46" s="26"/>
+      <c r="M46" s="24">
         <v>0.41666666666666669</v>
       </c>
       <c r="N46" s="6"/>
-      <c r="O46" s="70"/>
+      <c r="O46" s="23"/>
     </row>
     <row r="47" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F47" s="21">
         <v>5</v>
       </c>
-      <c r="G47" s="26">
+      <c r="G47" s="48">
         <v>4</v>
       </c>
-      <c r="H47" s="26"/>
+      <c r="H47" s="48"/>
       <c r="I47" s="21">
         <v>1</v>
       </c>
       <c r="J47" s="21">
         <v>3</v>
       </c>
-      <c r="K47" s="71">
+      <c r="K47" s="25">
         <v>43503</v>
       </c>
-      <c r="L47" s="72"/>
-      <c r="M47" s="73">
+      <c r="L47" s="26"/>
+      <c r="M47" s="24">
         <v>0.45885416666666662</v>
       </c>
       <c r="N47" s="6"/>
-      <c r="O47" s="70"/>
+      <c r="O47" s="23"/>
     </row>
     <row r="48" spans="6:22" x14ac:dyDescent="0.25">
       <c r="F48" s="21">
         <v>6</v>
       </c>
-      <c r="G48" s="26">
+      <c r="G48" s="48">
         <v>7</v>
       </c>
-      <c r="H48" s="26"/>
+      <c r="H48" s="48"/>
       <c r="I48" s="21">
         <v>3</v>
       </c>
       <c r="J48" s="21">
         <v>2</v>
       </c>
-      <c r="K48" s="71">
+      <c r="K48" s="25">
         <v>43898</v>
       </c>
-      <c r="L48" s="72"/>
+      <c r="L48" s="26"/>
       <c r="M48" s="20" t="s">
         <v>137</v>
       </c>
       <c r="N48" s="6"/>
-      <c r="O48" s="70"/>
+      <c r="O48" s="23"/>
     </row>
     <row r="49" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F49" s="21">
         <v>7</v>
       </c>
-      <c r="G49" s="26">
+      <c r="G49" s="48">
         <v>4</v>
       </c>
-      <c r="H49" s="26"/>
+      <c r="H49" s="48"/>
       <c r="I49" s="21">
         <v>1</v>
       </c>
       <c r="J49" s="21">
         <v>2</v>
       </c>
-      <c r="K49" s="71">
+      <c r="K49" s="25">
         <v>43899</v>
       </c>
-      <c r="L49" s="72"/>
-      <c r="M49" s="73">
+      <c r="L49" s="26"/>
+      <c r="M49" s="24">
         <v>0.45885416666666662</v>
       </c>
       <c r="N49" s="6"/>
-      <c r="O49" s="70"/>
+      <c r="O49" s="23"/>
     </row>
     <row r="50" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="N50" s="70"/>
-      <c r="O50" s="70"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
     </row>
     <row r="51" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="N51" s="70"/>
-      <c r="O51" s="70"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
     </row>
     <row r="52" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="N52" s="70"/>
-      <c r="O52" s="70"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="23"/>
     </row>
     <row r="53" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F53" s="56" t="s">
+      <c r="F53" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="G53" s="56"/>
-      <c r="H53" s="56"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
       <c r="I53" s="10"/>
       <c r="J53" t="s">
         <v>118</v>
       </c>
-      <c r="N53" s="70" t="s">
+      <c r="N53" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="O53" s="70"/>
+      <c r="O53" s="23"/>
     </row>
     <row r="54" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G54" s="55" t="s">
+      <c r="G54" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="H54" s="55"/>
+      <c r="H54" s="34"/>
     </row>
     <row r="55" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F55" s="2">
         <v>1</v>
       </c>
-      <c r="G55" s="53" t="s">
+      <c r="G55" s="46" t="s">
         <v>122</v>
       </c>
-      <c r="H55" s="54"/>
+      <c r="H55" s="47"/>
       <c r="K55" t="s">
         <v>117</v>
       </c>
@@ -2668,10 +2668,10 @@
       <c r="F56" s="2">
         <v>2</v>
       </c>
-      <c r="G56" s="53" t="s">
+      <c r="G56" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="H56" s="54"/>
+      <c r="H56" s="47"/>
       <c r="L56" t="s">
         <v>115</v>
       </c>
@@ -2683,10 +2683,10 @@
       <c r="F57" s="2">
         <v>3</v>
       </c>
-      <c r="G57" s="53" t="s">
+      <c r="G57" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="H57" s="54"/>
+      <c r="H57" s="47"/>
       <c r="M57" t="s">
         <v>114</v>
       </c>
@@ -2698,125 +2698,37 @@
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="F41:M41"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="S33:T33"/>
-    <mergeCell ref="S34:T34"/>
-    <mergeCell ref="U33:V33"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="M32:V32"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G57:H57"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="U29:V29"/>
-    <mergeCell ref="W29:X29"/>
-    <mergeCell ref="U28:V28"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W23:X23"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="W25:X25"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="W27:X27"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="U23:V23"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U25:V25"/>
-    <mergeCell ref="U26:V26"/>
-    <mergeCell ref="U27:V27"/>
-    <mergeCell ref="S27:T27"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="M20:X20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="S25:T25"/>
-    <mergeCell ref="S26:T26"/>
-    <mergeCell ref="S22:T22"/>
-    <mergeCell ref="S23:T23"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R15:S15"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R17:S17"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="M13:T13"/>
-    <mergeCell ref="W7:X7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="W9:X9"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="U9:V9"/>
-    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="F2:K2"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
     <mergeCell ref="I14:J14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="G16:H16"/>
@@ -2837,37 +2749,125 @@
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="F2:K2"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="M13:T13"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="W9:X9"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="S9:T9"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R15:S15"/>
+    <mergeCell ref="R16:S16"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="M20:X20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S27:T27"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U29:V29"/>
+    <mergeCell ref="W29:X29"/>
+    <mergeCell ref="U28:V28"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="W27:X27"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="U27:V27"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="M32:V32"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G57:H57"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="S33:T33"/>
+    <mergeCell ref="S34:T34"/>
+    <mergeCell ref="U33:V33"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="F41:M41"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="Q34:R34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{7413389C-42AD-4264-AF93-E4F1B4F7BAC2}"/>

</xml_diff>